<commit_message>
Handled errors, and filtered Business Titles
</commit_message>
<xml_diff>
--- a/RULES.xlsx
+++ b/RULES.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">PPM</t>
   </si>
   <si>
-    <t xml:space="preserve">Regional Category Manager</t>
+    <t xml:space="preserve">RCM</t>
   </si>
   <si>
     <t xml:space="preserve">Global Category Manager</t>
@@ -246,10 +246,10 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="2" style="1" width="14.27"/>

</xml_diff>

<commit_message>
Modified employees returned from functions
</commit_message>
<xml_diff>
--- a/RULES.xlsx
+++ b/RULES.xlsx
@@ -20,24 +20,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="34">
   <si>
     <t xml:space="preserve">Planner/Buyer</t>
   </si>
   <si>
-    <t xml:space="preserve">Procuremen Sourcing Leader or Nego Maker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S3L or Nego Maker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSC Manager</t>
+    <t xml:space="preserve">Procurement Sourcing Leader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S3L </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSC
+Manager</t>
   </si>
   <si>
     <t xml:space="preserve">PPM</t>
   </si>
   <si>
-    <t xml:space="preserve">RCM</t>
+    <t xml:space="preserve">Regional Category Manager</t>
   </si>
   <si>
     <t xml:space="preserve">Global Category Manager</t>
@@ -46,10 +47,11 @@
     <t xml:space="preserve">Global Category Director</t>
   </si>
   <si>
-    <t xml:space="preserve">NAM Regional Category Director</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VP Category Management</t>
+    <t xml:space="preserve">NAM
+Regional Category Director</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VP Category Manager</t>
   </si>
   <si>
     <t xml:space="preserve">Central Team</t>
@@ -245,18 +247,18 @@
   </sheetPr>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="2" style="1" width="14.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.63"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="53.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -292,7 +294,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -353,6 +355,9 @@
       <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="L4" s="1" t="s">
         <v>17</v>
       </c>
@@ -467,7 +472,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>29</v>
       </c>

</xml_diff>